<commit_message>
Back Milena Duarte / Documentacion Gina torres
</commit_message>
<xml_diff>
--- a/Documentacion/B02_Historia_Usuario.xlsx
+++ b/Documentacion/B02_Historia_Usuario.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mascotas\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E68AAC-D809-4F33-8A09-6EB8DB7938A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DC6875-8956-4E20-AFBF-F337D8013CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de usuario_Sprint0" sheetId="2" r:id="rId1"/>
     <sheet name="Historias de usuario_Sprint1" sheetId="3" r:id="rId2"/>
     <sheet name="Historias de usuario_Sprint2" sheetId="4" r:id="rId3"/>
-    <sheet name="Historias de usuario_Sprint3" sheetId="5" r:id="rId4"/>
-    <sheet name="Historias de usuario_Sprint4" sheetId="7" r:id="rId5"/>
+    <sheet name="Historias de usuario_Sprint3" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="70">
   <si>
     <t>HISTORIAS DE USUARIO</t>
   </si>
@@ -148,96 +147,18 @@
     <t>Observaciones: estaran como evidencia en la documentacion dentro del proyecto</t>
   </si>
   <si>
-    <t>Formulario Inicio de sesion en frontend</t>
-  </si>
-  <si>
-    <t>Observaciones: Creacion de formulario Inicio de sesion en frontend</t>
-  </si>
-  <si>
-    <t>Observaciones:  Creacion de formulario Registro / consultar mascotas en frontend</t>
-  </si>
-  <si>
     <t>Formulario Registro / consultar mascotas</t>
   </si>
   <si>
-    <t>Descripción: Yo como veterinario necesito acceder a la aplicación para poder ingresar los datos de la visita realizada a la mascota, esto con el fin de tener seguridad y solo ingrese el personal autorizado, esta debe tener un usuario y contraseña para garantizar seguridad, boton para su respectivo ingreso.</t>
-  </si>
-  <si>
-    <t>Descripción:   Yo como veterinario necesito registrar las mascotas a las que se le realiza la visita con esto para centrarlizar la informacion en una BD y asi mismo consultar esta informacion cuando sea requerida, se debe visualizar los datos como Nombre, color, especie, raza, dueño, veterinario y historia.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Formulario Registro propietario </t>
   </si>
   <si>
-    <t>Observaciones: Creacion de formulario Registro propietario en frontend</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como veterinario necesito registrar a un dueño para poder asignarlo a su mascota correspondiente para con esto identificarlo, es necesario que este formulario lleve el campo de correo</t>
-  </si>
-  <si>
-    <t>Observaciones: Creacion de formulario Registro veterinario en frontend</t>
-  </si>
-  <si>
     <t>Formulario Registro veterinario</t>
   </si>
   <si>
-    <t>Descripción: Yo como veterinario necesito registrar a un veterinario para poder asignarlo a la visita realizada a la mascota para con esto identificar quien lo atendio, es necesario que este formulario tenga el campo Tarjeta Profesional</t>
-  </si>
-  <si>
     <t xml:space="preserve">Formulario Visita </t>
   </si>
   <si>
-    <t>Observaciones: Creacion de formulario Visita en frontend</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como veterinario necesito poder registrar los datos correspondientes a la visita que se realizo a la mascota, este formulario debe tener los campos Fecha visita, Temperatura, peso, frecuencia respiratoria, frecuencia cardiaca, estado animo, recomendacion, veterinario</t>
-  </si>
-  <si>
-    <t>Backend de Inicio de sesion</t>
-  </si>
-  <si>
-    <t>Observaciones: Creacion de Backend de Inicio de sesion</t>
-  </si>
-  <si>
-    <t>Backend de Registro mascotas</t>
-  </si>
-  <si>
-    <t>Observaciones:  Creacion de Backend de Registro mascotas</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como desarrollador necesito ingresar un usuario y contraseña los cuales se conecten el frontend y la BD para asi validar su contraseña y dar ingreso a la aplicación.</t>
-  </si>
-  <si>
-    <t>Backend de  Registro propietario</t>
-  </si>
-  <si>
-    <t>Observaciones: Creacion de Backend de  Registro propietario</t>
-  </si>
-  <si>
-    <t>Backend de Registro veterinario</t>
-  </si>
-  <si>
-    <t>Observaciones: Creacion de Backend de Registro veterinario</t>
-  </si>
-  <si>
-    <t>Backend de Visita</t>
-  </si>
-  <si>
-    <t>Observaciones: Creacion de Backend de Visita</t>
-  </si>
-  <si>
-    <t>Descripción:   Yo como desarrollador necesito ingresar los datos de formulario visita a la BD para asi validar tener el historico necesario para poder realizar la relacion que tiene el visita con la mascota.</t>
-  </si>
-  <si>
-    <t>Descripción:   Yo como desarrollador necesito ingresar los datos del registro veterinario a la BD para asi validar tener el historico necesario para poder realizar la relacion que tiene con la mascota.</t>
-  </si>
-  <si>
-    <t>Descripción:   Yo como desarrollador necesito ingresar los datos del registro propietario a la BD para asi validar tener el historico necesario para poder realizar la relacion que tiene con la mascota.</t>
-  </si>
-  <si>
-    <t>Descripción:   Yo como desarrollador necesito ingresar los datos del registro mascota a la BD para asi validar tener el historico necesario para poder realizar la relacion que tiene con el dueño, veterinario y visita.</t>
-  </si>
-  <si>
     <t>Asignar un veterinario a una mascota</t>
   </si>
   <si>
@@ -253,43 +174,76 @@
     <t>Consultar listado de mascotas por veterinario</t>
   </si>
   <si>
-    <t>Observaciones: Consultar listado de mascotas por veterinario. Al consultar las mascotas, se podrán ver los datos de una mascota en particular.</t>
-  </si>
-  <si>
     <t>Consultar listado de mascotas por propietario</t>
   </si>
   <si>
-    <t>Observaciones: Consultar listado de mascotas por propietario. Al consultar las mascotas, se podrán ver los datos de una mascota en particular.</t>
-  </si>
-  <si>
-    <t>Observaciones: Asignar un veterinario a una mascota.</t>
-  </si>
-  <si>
-    <t>Observaciones:  Actualizar datos de paciente, mascota, veterinario</t>
-  </si>
-  <si>
     <t xml:space="preserve">Observaciones: Autenticación, consulta de historia clínica incluyendo las visitas, actualizar datos de visita. </t>
   </si>
   <si>
     <t xml:space="preserve">Autenticación, consulta de historia clínica </t>
   </si>
   <si>
-    <t>Descripción: Yo como desarrollador necesito asignar el veterinario a la mascota que atendio por medio del Backend</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como desarrollador necesito actualizar los datos propietario, mascota y veterinario por medio del Backend</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como desarrollador necesito registrar las visitas por medio del Backend</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como desarrollador necesito enlistar las mascotas por veterinario por medio del Backend</t>
-  </si>
-  <si>
-    <t>Descripción: Yo como desarrollador necesito enlistar las mascotas por propietario por medio del Backend</t>
-  </si>
-  <si>
-    <t>Descripción:   Yo como desarrollador necesito consultar la historia clinica y actualizar los datos de la visita por medio del Backend.</t>
+    <t>Descripción: Yo como veterinario necesito acceder a la aplicación para poder ingresar los datos de la visita realizada a la mascota, esto con el fin de tener seguridad y solo ingrese el personal autorizado.</t>
+  </si>
+  <si>
+    <t>Formulario Inicio de sesion</t>
+  </si>
+  <si>
+    <t>Observaciones:  En este formulario se debe visualizar los datos como Nombre, color, especie, raza, dueño, veterinario y historia.</t>
+  </si>
+  <si>
+    <t>Observaciones: En este formulario se debe visualizar un campo de usuario y contraseña para garantizar seguridad, boton para su respectivo ingreso.</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como veterinario necesito registrar a un dueño para poder asignarlo a su mascota correspondiente para con esto identificarlo.</t>
+  </si>
+  <si>
+    <t>Observaciones: Es necesario que este formulario lleve el campo de correo</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como veterinario necesito registrar a un veterinario para poder asignarlo a la visita realizada a la mascota para con esto identificar quien lo atendio.</t>
+  </si>
+  <si>
+    <t>Observaciones: Es necesario que este formulario tenga el campo Tarjeta Profesional del veterinario</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como veterinario necesito poder registrar los datos correspondientes a la visita que se realizo a la mascota.</t>
+  </si>
+  <si>
+    <t>Observaciones: Este formulario debe tener los campos Fecha visita, Temperatura, peso, frecuencia respiratoria, frecuencia cardiaca, estado animo, recomendacion, veterinario</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como veterinario necesito identificar el veterinario que atendio a la mascota.</t>
+  </si>
+  <si>
+    <t>Descripción:   Yo como veterinario necesito registrar las mascotas a las que se le realiza la visita con esto para centrarlizar la informacion y asi mismo consultar esta informacion cuando sea requerida</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como usuario necesito actualizar los datos propietario, mascota y veterinario</t>
+  </si>
+  <si>
+    <t>Observaciones:  los datos que se podran actualizar son los mismos de registro de cada perfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observaciones: </t>
+  </si>
+  <si>
+    <t>Descripción: Yo como veterinario necesito registrar las visitas realizadas a las mascotas</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como usuario necesito visualizar una lista de las mascotas por veterinario</t>
+  </si>
+  <si>
+    <t>Observaciones:  Al consultar las mascotas, se podrán ver los datos de una mascota en particular.</t>
+  </si>
+  <si>
+    <t>Descripción: Yo como usuario necesito visualizar una lista de las mascotas por propietario</t>
+  </si>
+  <si>
+    <t>Observaciones: Al consultar las mascotas, se podrán ver los datos de una mascota en particular.</t>
+  </si>
+  <si>
+    <t>Descripción:   Yo como usuario necesito consultar la historia clinica y actualizar los datos de la visita.</t>
   </si>
 </sst>
 </file>
@@ -462,14 +416,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -488,6 +434,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="12" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -721,17 +675,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="27"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -739,36 +693,36 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="27">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -793,7 +747,7 @@
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="12"/>
@@ -831,30 +785,30 @@
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
@@ -891,17 +845,17 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -909,36 +863,36 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="27">
         <v>2</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -963,7 +917,7 @@
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="12"/>
@@ -1001,56 +955,56 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="23"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="23"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
@@ -1061,17 +1015,17 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1079,36 +1033,36 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="27">
         <v>3</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="25"/>
       <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="18"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -1133,7 +1087,7 @@
       <c r="E39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G39" s="12"/>
@@ -1288,7 +1242,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55:G55"/>
+      <selection activeCell="B10" sqref="B10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1300,17 +1254,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="27"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1318,36 +1272,36 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="27">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1372,7 +1326,7 @@
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="16">
         <v>44652</v>
       </c>
       <c r="G7" s="12"/>
@@ -1410,30 +1364,30 @@
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
@@ -1470,17 +1424,17 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1488,36 +1442,36 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="27">
         <v>5</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -1542,7 +1496,7 @@
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="16">
         <v>44652</v>
       </c>
       <c r="G23" s="12"/>
@@ -1580,56 +1534,56 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="23"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="23"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
@@ -1640,17 +1594,17 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1658,36 +1612,36 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="27">
         <v>6</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="25"/>
       <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="18"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -1712,7 +1666,7 @@
       <c r="E39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="16">
         <v>44652</v>
       </c>
       <c r="G39" s="12"/>
@@ -1810,17 +1764,17 @@
       <c r="G48" s="9"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="27"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -1828,36 +1782,36 @@
       <c r="G50" s="9"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="26"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="27">
         <v>7</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="25"/>
       <c r="E52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F52" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G52" s="18"/>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="16"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="18"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="26"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
@@ -1882,7 +1836,7 @@
       <c r="E55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="16">
         <v>44652</v>
       </c>
       <c r="G55" s="12"/>
@@ -2051,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FF2534-B9C2-47DF-9C14-6D6E99696F76}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80:G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2064,17 +2018,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="27"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -2082,36 +2036,36 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="27">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="18"/>
+      <c r="F4" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -2136,7 +2090,7 @@
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="16">
         <v>44653</v>
       </c>
       <c r="G7" s="12"/>
@@ -2175,7 +2129,7 @@
     </row>
     <row r="10" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -2201,7 +2155,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2234,17 +2188,17 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2252,36 +2206,36 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="27">
         <v>5</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="18"/>
+      <c r="F20" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -2306,7 +2260,7 @@
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="16">
         <v>44653</v>
       </c>
       <c r="G23" s="12"/>
@@ -2345,7 +2299,7 @@
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -2370,30 +2324,30 @@
       <c r="G28" s="15"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
+      <c r="B29" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
@@ -2404,17 +2358,17 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -2422,36 +2376,36 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="27">
         <v>6</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="25"/>
       <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="18"/>
+      <c r="F36" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -2476,7 +2430,7 @@
       <c r="E39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="16">
         <v>44653</v>
       </c>
       <c r="G39" s="12"/>
@@ -2515,7 +2469,7 @@
     </row>
     <row r="42" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -2541,7 +2495,7 @@
     </row>
     <row r="45" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="13" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -2574,17 +2528,17 @@
       <c r="G48" s="9"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="27"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -2592,36 +2546,36 @@
       <c r="G50" s="9"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="26"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="27">
         <v>7</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="25"/>
       <c r="E52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G52" s="18"/>
+      <c r="F52" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="16"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="18"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="26"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
@@ -2646,7 +2600,7 @@
       <c r="E55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="16">
         <v>44653</v>
       </c>
       <c r="G55" s="12"/>
@@ -2685,7 +2639,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="13" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -2711,7 +2665,7 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="13" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -2744,17 +2698,17 @@
       <c r="G64" s="9"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="27"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
@@ -2762,36 +2716,36 @@
       <c r="G66" s="9"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="16"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="18"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="19">
+      <c r="C68" s="27">
         <v>7</v>
       </c>
-      <c r="D68" s="17"/>
+      <c r="D68" s="25"/>
       <c r="E68" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F68" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G68" s="18"/>
+      <c r="F68" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="26"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="18"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="26"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="5" t="s">
@@ -2816,7 +2770,7 @@
       <c r="E71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F71" s="20">
+      <c r="F71" s="16">
         <v>44653</v>
       </c>
       <c r="G71" s="12"/>
@@ -2855,7 +2809,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B74" s="13" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
@@ -2881,7 +2835,7 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="13" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
@@ -2927,11 +2881,6 @@
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="F72:G72"/>
-    <mergeCell ref="B58:G60"/>
-    <mergeCell ref="B61:G63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:G66"/>
-    <mergeCell ref="B67:G67"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="C54:D54"/>
@@ -2941,11 +2890,11 @@
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B58:G60"/>
+    <mergeCell ref="B61:G63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:G66"/>
+    <mergeCell ref="B67:G67"/>
     <mergeCell ref="B53:G53"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="F40:G40"/>
@@ -2953,11 +2902,11 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="B42:G44"/>
     <mergeCell ref="B45:G47"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F52:G52"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="C25:D25"/>
@@ -2966,17 +2915,17 @@
     <mergeCell ref="B29:G31"/>
     <mergeCell ref="B32:G32"/>
     <mergeCell ref="B33:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B10:G12"/>
-    <mergeCell ref="B13:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B19:G19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="C7:D7"/>
@@ -2985,972 +2934,28 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B10:G12"/>
+    <mergeCell ref="B13:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191BB820-D575-40DA-9668-5266F53B3A52}">
-  <dimension ref="A1:I81"/>
-  <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="7" width="19" customWidth="1"/>
-    <col min="8" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="16384" width="5.7109375" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="27"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="19">
-        <v>4</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="20">
-        <v>44654</v>
-      </c>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="28">
-        <v>5</v>
-      </c>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="28">
-        <v>5</v>
-      </c>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="19">
-        <v>5</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="20">
-        <v>44654</v>
-      </c>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="10">
-        <v>8</v>
-      </c>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="10">
-        <v>9</v>
-      </c>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
-    </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
-    </row>
-    <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
-    </row>
-    <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
-    </row>
-    <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="19">
-        <v>6</v>
-      </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="20">
-        <v>44654</v>
-      </c>
-      <c r="G39" s="12"/>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="10">
-        <v>8</v>
-      </c>
-      <c r="G40" s="12"/>
-    </row>
-    <row r="41" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="10">
-        <v>9</v>
-      </c>
-      <c r="G41" s="12"/>
-    </row>
-    <row r="42" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="15"/>
-    </row>
-    <row r="43" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="15"/>
-    </row>
-    <row r="44" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="15"/>
-    </row>
-    <row r="45" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="13"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="15"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="15"/>
-    </row>
-    <row r="48" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="27"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="9"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="19">
-        <v>7</v>
-      </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G52" s="18"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="16"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="18"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F55" s="20">
-        <v>44654</v>
-      </c>
-      <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="10">
-        <v>8</v>
-      </c>
-      <c r="G56" s="12"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="10">
-        <v>9</v>
-      </c>
-      <c r="G57" s="12"/>
-    </row>
-    <row r="58" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="15"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B59" s="13"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="15"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B60" s="13"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="15"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="15"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="13"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="15"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B63" s="13"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="15"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B64" s="7"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="9"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="27"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="9"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="16"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="18"/>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B68" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="19">
-        <v>7</v>
-      </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F68" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G68" s="18"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="18"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B70" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="6"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B71" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" s="20">
-        <v>44654</v>
-      </c>
-      <c r="G71" s="12"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B72" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="11"/>
-      <c r="E72" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="10">
-        <v>8</v>
-      </c>
-      <c r="G72" s="12"/>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B73" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="11"/>
-      <c r="E73" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="10">
-        <v>9</v>
-      </c>
-      <c r="G73" s="12"/>
-    </row>
-    <row r="74" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="15"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B75" s="13"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="15"/>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B76" s="13"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="15"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B77" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="15"/>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B78" s="13"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="15"/>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B79" s="13"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="15"/>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B80" s="7"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="9"/>
-    </row>
-    <row r="81" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="B74:G76"/>
-    <mergeCell ref="B77:G79"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="B58:G60"/>
-    <mergeCell ref="B61:G63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:G66"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:G44"/>
-    <mergeCell ref="B45:G47"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B26:G28"/>
-    <mergeCell ref="B29:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G34"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B10:G12"/>
-    <mergeCell ref="B13:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="C6:D6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA29D24-3E44-4AE1-B701-198E1AE3FC5E}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93:G95"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3965,17 +2970,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="27"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -3983,36 +2988,36 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="27">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="18"/>
+      <c r="F4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4037,7 +3042,7 @@
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="16">
         <v>44654</v>
       </c>
       <c r="G7" s="12"/>
@@ -4076,7 +3081,7 @@
     </row>
     <row r="10" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -4102,7 +3107,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4135,17 +3140,17 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -4153,36 +3158,36 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="27">
         <v>5</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="18"/>
+      <c r="F20" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -4207,7 +3212,7 @@
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="16">
         <v>44654</v>
       </c>
       <c r="G23" s="12"/>
@@ -4246,7 +3251,7 @@
     </row>
     <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -4271,30 +3276,30 @@
       <c r="G28" s="15"/>
     </row>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
+      <c r="B29" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="23"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
@@ -4305,17 +3310,17 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -4323,36 +3328,36 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="27">
         <v>6</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="25"/>
       <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" s="18"/>
+      <c r="F36" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -4377,7 +3382,7 @@
       <c r="E39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="20">
+      <c r="F39" s="16">
         <v>44654</v>
       </c>
       <c r="G39" s="12"/>
@@ -4416,7 +3421,7 @@
     </row>
     <row r="42" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -4442,7 +3447,7 @@
     </row>
     <row r="45" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="13" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -4475,17 +3480,17 @@
       <c r="G48" s="9"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="27"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -4493,36 +3498,36 @@
       <c r="G50" s="9"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="26"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="27">
         <v>7</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="25"/>
       <c r="E52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G52" s="18"/>
+      <c r="F52" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="16"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="18"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="26"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="s">
@@ -4547,7 +3552,7 @@
       <c r="E55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="16">
         <v>44654</v>
       </c>
       <c r="G55" s="12"/>
@@ -4586,7 +3591,7 @@
     </row>
     <row r="58" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="13" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -4612,7 +3617,7 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -4645,17 +3650,17 @@
       <c r="G64" s="9"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="27"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
@@ -4663,36 +3668,36 @@
       <c r="G66" s="9"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="16"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="18"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="19">
+      <c r="C68" s="27">
         <v>7</v>
       </c>
-      <c r="D68" s="17"/>
+      <c r="D68" s="25"/>
       <c r="E68" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F68" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G68" s="18"/>
+      <c r="F68" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G68" s="26"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="18"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="26"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="5" t="s">
@@ -4717,7 +3722,7 @@
       <c r="E71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F71" s="20">
+      <c r="F71" s="16">
         <v>44654</v>
       </c>
       <c r="G71" s="12"/>
@@ -4756,7 +3761,7 @@
     </row>
     <row r="74" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="13" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
@@ -4782,7 +3787,7 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
@@ -4815,17 +3820,17 @@
       <c r="G80" s="9"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B81" s="24" t="s">
+      <c r="B81" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="26"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="22"/>
     </row>
     <row r="82" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="27"/>
+      <c r="B82" s="23"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
@@ -4833,36 +3838,36 @@
       <c r="G82" s="9"/>
     </row>
     <row r="83" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="16"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="18"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="26"/>
     </row>
     <row r="84" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C84" s="19">
+      <c r="C84" s="27">
         <v>7</v>
       </c>
-      <c r="D84" s="17"/>
+      <c r="D84" s="25"/>
       <c r="E84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F84" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G84" s="18"/>
+      <c r="F84" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G84" s="26"/>
     </row>
     <row r="85" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="16"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="18"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="26"/>
     </row>
     <row r="86" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="5" t="s">
@@ -4887,7 +3892,7 @@
       <c r="E87" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F87" s="20">
+      <c r="F87" s="16">
         <v>44654</v>
       </c>
       <c r="G87" s="12"/>
@@ -4926,7 +3931,7 @@
     </row>
     <row r="90" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C90" s="14"/>
       <c r="D90" s="14"/>
@@ -4952,7 +3957,7 @@
     </row>
     <row r="93" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="13" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="C93" s="14"/>
       <c r="D93" s="14"/>
@@ -4995,11 +4000,6 @@
     <mergeCell ref="F89:G89"/>
     <mergeCell ref="B90:G92"/>
     <mergeCell ref="B93:G95"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="F87:G87"/>
     <mergeCell ref="C73:D73"/>
@@ -5008,17 +4008,17 @@
     <mergeCell ref="B77:G79"/>
     <mergeCell ref="B80:G80"/>
     <mergeCell ref="B81:G82"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="C86:D86"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="F71:G71"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="F72:G72"/>
-    <mergeCell ref="B58:G60"/>
-    <mergeCell ref="B61:G63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:G66"/>
-    <mergeCell ref="B67:G67"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="F68:G68"/>
     <mergeCell ref="C54:D54"/>
@@ -5028,11 +4028,11 @@
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B58:G60"/>
+    <mergeCell ref="B61:G63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:G66"/>
+    <mergeCell ref="B67:G67"/>
     <mergeCell ref="B53:G53"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="F40:G40"/>
@@ -5040,11 +4040,11 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="B42:G44"/>
     <mergeCell ref="B45:G47"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F52:G52"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="C25:D25"/>
@@ -5053,17 +4053,17 @@
     <mergeCell ref="B29:G31"/>
     <mergeCell ref="B32:G32"/>
     <mergeCell ref="B33:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B10:G12"/>
-    <mergeCell ref="B13:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G18"/>
-    <mergeCell ref="B19:G19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="C7:D7"/>
@@ -5072,12 +4072,17 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B10:G12"/>
+    <mergeCell ref="B13:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>